<commit_message>
thêm chức năng xuất file điểm toàn khóa
</commit_message>
<xml_diff>
--- a/public/upload/file_mau/bang_danh_gia_ren_luyen_sv_toan_khoa.xlsx
+++ b/public/upload/file_mau/bang_danh_gia_ren_luyen_sv_toan_khoa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\danh gia ren luyen thay hung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Laravel\luanvantotnghiep\public\upload\file_mau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>BỘ GIÁO DỤC VÀ ĐÀO TẠO</t>
   </si>
@@ -67,9 +67,6 @@
     </r>
   </si>
   <si>
-    <t>thai duc</t>
-  </si>
-  <si>
     <t>Chi tiết kết quả đánh giá rèn luyện toàn khóa học:</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>MSSV:</t>
   </si>
   <si>
-    <t>dh514124</t>
-  </si>
-  <si>
     <t>Lớp:</t>
   </si>
   <si>
@@ -100,7 +94,22 @@
     <t>ĐIỂM HỌC KỲ II</t>
   </si>
   <si>
-    <t>Năm học</t>
+    <t>Xếp loại rèn luyện toàn khóa học:</t>
+  </si>
+  <si>
+    <t>Điểm trung bình rèn luyện toàn khóa học:</t>
+  </si>
+  <si>
+    <t>Tp. Hồ Chí Minh, ngày … tháng … năm …</t>
+  </si>
+  <si>
+    <t>Hiệu trưởng</t>
+  </si>
+  <si>
+    <t>PGS. TS. Cao Hào Thi</t>
+  </si>
+  <si>
+    <t>GHI CHÚ</t>
   </si>
 </sst>
 </file>
@@ -158,7 +167,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -170,21 +179,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -202,6 +196,59 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -211,13 +258,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -226,15 +294,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,380 +586,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" customWidth="1"/>
     <col min="2" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="6"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="6"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
     </row>
     <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="29">
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="A5:L5"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="G22:L22"/>
+    <mergeCell ref="H28:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>